<commit_message>
Creacion de entidades y DbContext
</commit_message>
<xml_diff>
--- a/Base de Datos.xlsx
+++ b/Base de Datos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Proyectos .Net\Proyecto-Entrevista-Brasil\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Proyectos .Net\Prueba-Practica-Autoestrada\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -56,9 +56,6 @@
     <t>P001</t>
   </si>
   <si>
-    <t>Leche deslactosada</t>
-  </si>
-  <si>
     <t>Nombre</t>
   </si>
   <si>
@@ -156,6 +153,9 @@
   </si>
   <si>
     <t>Salchicha Ranchera 12 unidades</t>
+  </si>
+  <si>
+    <t>Leche deslactosada 1litro</t>
   </si>
 </sst>
 </file>
@@ -187,7 +187,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -210,26 +210,14 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -517,7 +505,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -534,20 +522,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="I1" s="5" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="I1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -572,7 +560,7 @@
         <v>7</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>2</v>
@@ -586,10 +574,10 @@
         <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D3" s="2">
         <v>44876</v>
@@ -598,16 +586,16 @@
         <v>45240</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="L3" s="1">
         <v>3006338992</v>
@@ -615,13 +603,13 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="D4" s="2">
         <v>44844</v>
@@ -630,16 +618,16 @@
         <v>45239</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="L4" s="1">
         <v>3118989898</v>
@@ -647,13 +635,13 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="D5" s="2">
         <v>44846</v>
@@ -661,31 +649,31 @@
       <c r="E5" s="2">
         <v>45272</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J5" s="4" t="s">
+      <c r="K5" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>23</v>
       </c>
       <c r="L5" s="1">
         <v>3215658989</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>16</v>
+      <c r="C6" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="D6" s="2">
         <v>44876</v>
@@ -693,31 +681,31 @@
       <c r="E6" s="2">
         <v>45242</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J6" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="I6" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J6" s="4" t="s">
+      <c r="K6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="K6" s="4" t="s">
+      <c r="L6" s="3">
+        <v>3158987744</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="L6" s="4">
-        <v>3158987744</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>16</v>
+      <c r="C7" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="D7" s="2">
         <v>44844</v>
@@ -726,30 +714,30 @@
         <v>45239</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J7" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="K7" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="L7" s="3">
         <v>3125658651</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>16</v>
+      <c r="C8" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="D8" s="2">
         <v>44846</v>
@@ -757,19 +745,19 @@
       <c r="E8" s="2">
         <v>45272</v>
       </c>
-      <c r="F8" s="4" t="s">
-        <v>21</v>
+      <c r="F8" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="C9" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D9" s="2">
         <v>44876</v>
@@ -778,18 +766,18 @@
         <v>45240</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="4" t="s">
+      <c r="A10" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>16</v>
+      <c r="B10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="D10" s="2">
         <v>44876</v>
@@ -797,19 +785,19 @@
       <c r="E10" s="2">
         <v>45242</v>
       </c>
-      <c r="F10" s="4" t="s">
-        <v>28</v>
+      <c r="F10" s="3" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>43</v>
-      </c>
       <c r="C11" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D11" s="2">
         <v>44845</v>
@@ -818,7 +806,7 @@
         <v>45272</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>